<commit_message>
community & block wise topup reports
</commit_message>
<xml_diff>
--- a/src/main/resources/PAYGTL_LORA_BLE Work Details.xlsx
+++ b/src/main/resources/PAYGTL_LORA_BLE Work Details.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t>Module No.</t>
   </si>
@@ -898,7 +898,7 @@
   <dimension ref="B1:G57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,7 +955,7 @@
       <c r="C5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="20">
         <v>1</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -975,6 +975,9 @@
       <c r="F6" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="G6" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="20">
@@ -988,6 +991,9 @@
       </c>
       <c r="F7" s="4" t="s">
         <v>33</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -1346,7 +1352,7 @@
       </c>
     </row>
     <row r="49" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="5">
+      <c r="B49" s="21">
         <v>12</v>
       </c>
       <c r="C49" s="6" t="s">

</xml_diff>